<commit_message>
Update experiment vs model comparison figure
</commit_message>
<xml_diff>
--- a/DunData.xlsx
+++ b/DunData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turbo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\paramFreePea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67843841-52BF-4D03-8565-B1A8A0556BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B781219-A2DB-432C-AC06-1EFA5CA1B7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6461AC70-E17B-47DC-AAFD-74096596C3F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6461AC70-E17B-47DC-AAFD-74096596C3F9}"/>
   </bookViews>
   <sheets>
     <sheet name="CK" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="109">
   <si>
     <t>Description</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>RMS5r2</t>
+  </si>
+  <si>
+    <t>This data is used by the code to compile and process the different results across genetic perturbation experiments, for pea plant branching behaviour and levels of phytohormone and gene expression. Perturbations include the use of genotypically distinct shoot and root and/or genotypically distinct grafts within the shoot or root. A detailed description of this data, including original sources, is provided in the article from which this data was taken:</t>
+  </si>
+  <si>
+    <t>E. A. Dun, J. Hanan, C. A. Beveridge, Computational modeling and molecular physiology experiments reveal new insights into shoot branching in pea, The Plant Cell 21 (2009) 3459–3472.</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +427,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,9 +452,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +492,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -585,7 +598,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD1163-5518-4407-9AAF-2EF94489533A}">
-  <dimension ref="B2:AB24"/>
+  <dimension ref="B2:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,7 +2443,150 @@
         <v>24</v>
       </c>
     </row>
+    <row r="26" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+    <row r="29" spans="2:26" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B30:Z30"/>
+    <mergeCell ref="B26:Z28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>